<commit_message>
Matched simulation notebook to Excel tests
</commit_message>
<xml_diff>
--- a/youtube simulation/Weighted Sum for Rankings - Test.xlsx
+++ b/youtube simulation/Weighted Sum for Rankings - Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sasha Rabeno\Desktop\Spring 2023\ENGR 050\repo\tools-of-justice\youtube simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBA7C5C-553C-4E09-B7F0-869BE9C1D34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CE10E6-31FF-4C12-AB6F-1227C6E46305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{DAB9F06C-9FE5-4E61-A144-89B06CA55864}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Weight</t>
   </si>
@@ -242,6 +242,24 @@
   </si>
   <si>
     <t>#3</t>
+  </si>
+  <si>
+    <t>normalize everything</t>
+  </si>
+  <si>
+    <t>divide whole column by largest</t>
+  </si>
+  <si>
+    <t>Normalized 1</t>
+  </si>
+  <si>
+    <t>Normalized 2</t>
+  </si>
+  <si>
+    <t>Normalized 3</t>
+  </si>
+  <si>
+    <t>Normalized Value</t>
   </si>
 </sst>
 </file>
@@ -333,9 +351,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -358,6 +373,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,14 +877,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED79DB5-313B-462E-B2F2-499DD0084D05}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
@@ -918,27 +937,27 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <f>C10*B2</f>
+      <c r="B3" s="6">
+        <f>C15*B2</f>
         <v>9.4</v>
       </c>
-      <c r="C3" s="7">
-        <f>C11*C2</f>
+      <c r="C3" s="6">
+        <f>C16*C2</f>
         <v>117325.5</v>
       </c>
-      <c r="D3" s="7">
-        <f>C12*D2</f>
+      <c r="D3" s="6">
+        <f>C17*D2</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="E3" s="7">
-        <f>C13*E2</f>
+      <c r="E3" s="6">
+        <f>C18*E2</f>
         <v>0.105</v>
       </c>
-      <c r="F3" s="7">
-        <f>SUM(B3:E3)</f>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F8" si="0">SUM(B3:E3)</f>
         <v>117335.05499999999</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -949,27 +968,27 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
-        <f>D10*B2</f>
+      <c r="B4" s="8">
+        <f>D15*B2</f>
         <v>9.4</v>
       </c>
-      <c r="C4" s="9">
-        <f>C2*D11</f>
+      <c r="C4" s="8">
+        <f>C2*D16</f>
         <v>139485.29999999999</v>
       </c>
-      <c r="D4" s="9">
-        <f>D2*D12</f>
+      <c r="D4" s="8">
+        <f>D2*D17</f>
         <v>0.2</v>
       </c>
-      <c r="E4" s="9">
-        <f>E2*D13</f>
+      <c r="E4" s="8">
+        <f>E2*D18</f>
         <v>0.06</v>
       </c>
-      <c r="F4" s="9">
-        <f>SUM(B4:E4)</f>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
         <v>139494.96</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -980,27 +999,27 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11">
-        <f>B2*E10</f>
+      <c r="B5" s="10">
+        <f>B2*E15</f>
         <v>3.8000000000000003</v>
       </c>
-      <c r="C5" s="11">
-        <f>C2*E11</f>
+      <c r="C5" s="10">
+        <f>C2*E16</f>
         <v>81029.7</v>
       </c>
-      <c r="D5" s="11">
-        <f>D2*E12</f>
+      <c r="D5" s="10">
+        <f>D2*E17</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="E5" s="11">
-        <f>E2*E13</f>
+      <c r="E5" s="10">
+        <f>E2*E18</f>
         <v>0.105</v>
       </c>
-      <c r="F5" s="17">
-        <f>SUM(B5:E5)</f>
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
         <v>81033.654999999999</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1010,223 +1029,394 @@
         <v>0.8</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6">
+        <f>B3/MAX(B$3:B$5)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" ref="C6:E6" si="1">C3/MAX(C$3:C$5)</f>
+        <v>0.84113164613045255</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.25000000000000022</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="0"/>
+        <v>3.091131646130453</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" ref="B7:E8" si="2">B4/MAX(B$3:B$5)</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="2"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>3.5714285714285712</v>
+      </c>
+    </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.4042553191489362</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.5809192796660293</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.25000000000000022</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
+        <v>2.2351745988149658</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>832170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="H13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C15" s="6">
         <f>ABS(I11-I3)</f>
         <v>47</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D15" s="8">
         <f>ABS(I19-I3)</f>
         <v>47</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E15" s="10">
         <f>ABS(I27-I3)</f>
         <v>19</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C16" s="6">
         <f>ABS(I4-I12)</f>
         <v>782170</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D16" s="8">
         <f>ABS(I4-I20)</f>
         <v>929902</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E16" s="10">
         <f>ABS(I4-I28)</f>
         <v>540198</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C17" s="6">
         <f>ABS(I5-I13)</f>
         <v>0.10000000000000009</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D17" s="8">
         <f>ABS(I5-I21)</f>
         <v>0.4</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E17" s="10">
         <f>ABS(I5-I29)</f>
         <v>0.10000000000000009</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12">
-        <v>832170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C18" s="6">
         <f>I13</f>
         <v>0.7</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D18" s="8">
         <f>I21</f>
         <v>0.4</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E18" s="10">
         <f>I29</f>
         <v>0.7</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19">
         <v>13</v>
       </c>
-      <c r="I13">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B16" s="16" t="s">
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>979902</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B21" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D21" s="16">
         <f>MIN(F3:F5)</f>
         <v>81033.654999999999</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E21" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C17" s="5" t="s">
+      <c r="H21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D22" s="20">
         <f>F3</f>
         <v>117335.05499999999</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C18" s="5" t="s">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D23" s="21">
         <f>MAX(F3:F5)</f>
         <v>139494.96</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="H19" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="H20" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20">
-        <v>979902</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="H21" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="H26" s="12" t="s">
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H26" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="H27" s="13" t="s">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H27" s="12" t="s">
         <v>11</v>
       </c>
       <c r="I27">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="H28" s="13" t="s">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C28" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="H28" s="12" t="s">
         <v>12</v>
       </c>
       <c r="I28">
         <v>590198</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="H29" s="13" t="s">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>13</v>
       </c>
       <c r="I29">
         <v>0.7</v>
       </c>
     </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="6">
+        <f>C15/MAX($C$15:$E$15)</f>
+        <v>1</v>
+      </c>
+      <c r="D30" s="8">
+        <f t="shared" ref="D30:E30" si="3">D15/MAX($C$15:$E$15)</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="3"/>
+        <v>0.40425531914893614</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="6">
+        <f>C16/MAX($C$16:$E$16)</f>
+        <v>0.84113164613045244</v>
+      </c>
+      <c r="D31" s="8">
+        <f>D16/MAX($C$16:$E$16)</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" ref="D31:E31" si="4">E16/MAX($C$16:$E$16)</f>
+        <v>0.5809192796660293</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="6">
+        <f>C17/MAX($C$17:$E$17)</f>
+        <v>0.25000000000000022</v>
+      </c>
+      <c r="D32" s="8">
+        <f t="shared" ref="D32:E32" si="5">D17/MAX($C$17:$E$17)</f>
+        <v>1</v>
+      </c>
+      <c r="E32" s="10">
+        <f t="shared" si="5"/>
+        <v>0.25000000000000022</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="6">
+        <f>C18/MAX($C$18:$E$18)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="8">
+        <f t="shared" ref="D33:E33" si="6">D18/MAX($C$18:$E$18)</f>
+        <v>0.57142857142857151</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C8:E8"/>
+  <mergeCells count="2">
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>